<commit_message>
add new column amplicon_name in submission spreadsheet in tabs amplicon and desirededitedsequence; create new output for frequency of desired edited sequence called amplicount_desired_edits.csv and remove these sequences from the general output amplicount.csv; fix issue when variant is WT when plotting; update submission spreadsheets
</commit_message>
<xml_diff>
--- a/data/GEP00005/GEP00005V3.xlsx
+++ b/data/GEP00005/GEP00005V3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="736"/>
+    <workbookView xWindow="2460" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="736" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="12" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="500">
   <si>
     <t>description</t>
   </si>
@@ -2127,6 +2127,9 @@
       </rPr>
       <t>Guide@name</t>
     </r>
+  </si>
+  <si>
+    <t>amplicon_name</t>
   </si>
 </sst>
 </file>
@@ -2262,7 +2265,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="201">
+  <cellStyleXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2464,8 +2467,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2494,8 +2499,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="201">
+  <cellStyles count="203">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2595,6 +2601,7 @@
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="42" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2695,10 +2702,1394 @@
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="41" builtinId="15"/>
   </cellStyles>
-  <dxfs count="130">
+  <dxfs count="132">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2992,19 +4383,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3082,6 +4460,19 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
         <strike val="0"/>
@@ -3491,1359 +4882,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
         <color auto="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
@@ -4865,9 +4903,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table264" displayName="Table264" ref="A4:C12" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="45"/>
-    <tableColumn id="2" name="Column names" dataDxfId="44"/>
-    <tableColumn id="3" name="Description" dataDxfId="43"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="131"/>
+    <tableColumn id="2" name="Column names" dataDxfId="130"/>
+    <tableColumn id="3" name="Description" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4876,9 +4914,9 @@
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table5073" displayName="Table5073" ref="A13:C13" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="8" dataDxfId="7"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="6" dataDxfId="5"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="4" dataDxfId="3"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="94" dataDxfId="93"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="92" dataDxfId="91"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="90" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4887,116 +4925,117 @@
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table1274" displayName="Table1274" ref="A73:C76" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="2"/>
-    <tableColumn id="2" name="Column names" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="88"/>
+    <tableColumn id="2" name="Column names" dataDxfId="87"/>
+    <tableColumn id="3" name="Description" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table20" displayName="Table20" ref="A1:G10" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
   <tableColumns count="7">
-    <tableColumn id="1" name="target_name" dataDxfId="127"/>
-    <tableColumn id="2" name="target_genome" dataDxfId="126"/>
-    <tableColumn id="3" name="target_gene_id" dataDxfId="125"/>
-    <tableColumn id="4" name="target_chrom" dataDxfId="124"/>
-    <tableColumn id="5" name="target_start" dataDxfId="123"/>
-    <tableColumn id="6" name="target_end" dataDxfId="122"/>
-    <tableColumn id="7" name="target_strand" dataDxfId="121"/>
+    <tableColumn id="1" name="target_name" dataDxfId="83"/>
+    <tableColumn id="2" name="target_genome" dataDxfId="82"/>
+    <tableColumn id="3" name="target_gene_id" dataDxfId="81"/>
+    <tableColumn id="4" name="target_chrom" dataDxfId="80"/>
+    <tableColumn id="5" name="target_start" dataDxfId="79"/>
+    <tableColumn id="6" name="target_end" dataDxfId="78"/>
+    <tableColumn id="7" name="target_strand" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" headerRowDxfId="120" dataDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table37" displayName="Table37" ref="H1:H10" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
   <tableColumns count="1">
-    <tableColumn id="1" name="target_description" dataDxfId="118"/>
+    <tableColumn id="1" name="target_description" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table21" displayName="Table21" ref="A1:C10" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <tableColumns count="3">
-    <tableColumn id="1" name="target_name" dataDxfId="115"/>
-    <tableColumn id="2" name="guide_name" dataDxfId="114"/>
-    <tableColumn id="3" name="guide_sequence" dataDxfId="113"/>
+    <tableColumn id="1" name="target_name" dataDxfId="71"/>
+    <tableColumn id="2" name="guide_name" dataDxfId="70"/>
+    <tableColumn id="3" name="guide_sequence" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="D1:G10" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <tableColumns count="4">
-    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="110"/>
-    <tableColumn id="2" name="guide_activity" dataDxfId="109"/>
-    <tableColumn id="3" name="guide_exon" dataDxfId="108"/>
-    <tableColumn id="4" name="guide_nuclease" dataDxfId="107"/>
+    <tableColumn id="1" name="guide_pam_sequence" dataDxfId="66"/>
+    <tableColumn id="2" name="guide_activity" dataDxfId="65"/>
+    <tableColumn id="3" name="guide_exon" dataDxfId="64"/>
+    <tableColumn id="4" name="guide_nuclease" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:M9" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
-  <tableColumns count="13">
-    <tableColumn id="1" name="guide_name" dataDxfId="104"/>
-    <tableColumn id="2" name="experiment_type" dataDxfId="103"/>
-    <tableColumn id="3" name="guide_location" dataDxfId="102"/>
-    <tableColumn id="4" name="guide_strand" dataDxfId="101"/>
-    <tableColumn id="5" name="is_on_target" dataDxfId="100"/>
-    <tableColumn id="6" name="dna_feature" dataDxfId="99"/>
-    <tableColumn id="7" name="chrom" dataDxfId="98"/>
-    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="97"/>
-    <tableColumn id="9" name="forward_primer_start" dataDxfId="96"/>
-    <tableColumn id="10" name="forward_primer_end" dataDxfId="95"/>
-    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="94"/>
-    <tableColumn id="12" name="reverse_primer_start" dataDxfId="93"/>
-    <tableColumn id="13" name="reverse_primer_end" dataDxfId="92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="A1:N9" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+  <tableColumns count="14">
+    <tableColumn id="14" name="amplicon_name" dataDxfId="1"/>
+    <tableColumn id="1" name="guide_name" dataDxfId="60"/>
+    <tableColumn id="2" name="experiment_type" dataDxfId="59"/>
+    <tableColumn id="3" name="guide_location" dataDxfId="58"/>
+    <tableColumn id="4" name="guide_strand" dataDxfId="57"/>
+    <tableColumn id="5" name="is_on_target" dataDxfId="56"/>
+    <tableColumn id="6" name="dna_feature" dataDxfId="55"/>
+    <tableColumn id="7" name="chrom" dataDxfId="54"/>
+    <tableColumn id="8" name="forward_primer_sequence" dataDxfId="53"/>
+    <tableColumn id="9" name="forward_primer_start" dataDxfId="52"/>
+    <tableColumn id="10" name="forward_primer_end" dataDxfId="51"/>
+    <tableColumn id="11" name="reverse_primer_sequence" dataDxfId="50"/>
+    <tableColumn id="12" name="reverse_primer_start" dataDxfId="49"/>
+    <tableColumn id="13" name="reverse_primer_end" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="N1:O9" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="O1:P9" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <tableColumns count="2">
-    <tableColumn id="1" name="score" dataDxfId="89"/>
-    <tableColumn id="2" name="description" dataDxfId="88"/>
+    <tableColumn id="1" name="score" dataDxfId="45"/>
+    <tableColumn id="2" name="description" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:C475" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="A1:C475" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <tableColumns count="3">
-    <tableColumn id="1" name="layout_id" dataDxfId="85"/>
-    <tableColumn id="2" name="well_position" dataDxfId="84"/>
-    <tableColumn id="13" name="sequencing_barcode" dataDxfId="83"/>
+    <tableColumn id="1" name="layout_id" dataDxfId="41"/>
+    <tableColumn id="2" name="well_position" dataDxfId="40"/>
+    <tableColumn id="13" name="sequencing_barcode" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="D1:M475" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="D1:M475" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <tableColumns count="10">
-    <tableColumn id="1" name="sequencing_sample_name" dataDxfId="80"/>
-    <tableColumn id="2" name="sequencing_dna_source" dataDxfId="79"/>
-    <tableColumn id="3" name="sequencing_library_type" dataDxfId="78"/>
-    <tableColumn id="4" name="sequencing_project_id" dataDxfId="77"/>
-    <tableColumn id="5" name="cell_line_name" dataDxfId="76"/>
-    <tableColumn id="6" name="cell_pool" dataDxfId="75"/>
-    <tableColumn id="7" name="clone_name" dataDxfId="74"/>
-    <tableColumn id="8" name="content_type" dataDxfId="73"/>
-    <tableColumn id="9" name="is_control" dataDxfId="72"/>
-    <tableColumn id="10" name="replicate_group" dataDxfId="71"/>
+    <tableColumn id="1" name="sequencing_sample_name" dataDxfId="36"/>
+    <tableColumn id="2" name="sequencing_dna_source" dataDxfId="35"/>
+    <tableColumn id="3" name="sequencing_library_type" dataDxfId="34"/>
+    <tableColumn id="4" name="sequencing_project_id" dataDxfId="33"/>
+    <tableColumn id="5" name="cell_line_name" dataDxfId="32"/>
+    <tableColumn id="6" name="cell_pool" dataDxfId="31"/>
+    <tableColumn id="7" name="clone_name" dataDxfId="30"/>
+    <tableColumn id="8" name="content_type" dataDxfId="29"/>
+    <tableColumn id="9" name="is_control" dataDxfId="28"/>
+    <tableColumn id="10" name="replicate_group" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5005,58 +5044,59 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table365" displayName="Table365" ref="A14:C18" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="42"/>
-    <tableColumn id="2" name="Column names" dataDxfId="41"/>
-    <tableColumn id="3" name="Description" dataDxfId="40"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="128"/>
+    <tableColumn id="2" name="Column names" dataDxfId="127"/>
+    <tableColumn id="3" name="Description" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:D6" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="51" name="Table51" displayName="Table51" ref="A1:D6" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <tableColumns count="4">
-    <tableColumn id="1" name="layout_id" dataDxfId="68"/>
-    <tableColumn id="2" name="plate_name" dataDxfId="67"/>
-    <tableColumn id="5" name="plate_barcode" dataDxfId="66"/>
-    <tableColumn id="4" name="plate_description" dataDxfId="65"/>
+    <tableColumn id="1" name="layout_id" dataDxfId="24"/>
+    <tableColumn id="2" name="plate_name" dataDxfId="23"/>
+    <tableColumn id="5" name="plate_barcode" dataDxfId="22"/>
+    <tableColumn id="4" name="plate_description" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:D31" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A1:D31" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <tableColumns count="4">
-    <tableColumn id="1" name="guide_name" dataDxfId="62"/>
-    <tableColumn id="2" name="is_off_target_coding_region" dataDxfId="61"/>
-    <tableColumn id="3" name="number_of_mismatches" dataDxfId="60"/>
-    <tableColumn id="4" name="number_of_off_targets" dataDxfId="59"/>
+    <tableColumn id="1" name="guide_name" dataDxfId="18"/>
+    <tableColumn id="2" name="is_off_target_coding_region" dataDxfId="17"/>
+    <tableColumn id="3" name="number_of_mismatches" dataDxfId="16"/>
+    <tableColumn id="4" name="number_of_off_targets" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1163" displayName="Table1163" ref="A1:B9" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <tableColumns count="2">
-    <tableColumn id="1" name="sequence_name" dataDxfId="49" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="sequence" dataDxfId="48" dataCellStyle="Normal"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1163" displayName="Table1163" ref="A1:C9" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <tableColumns count="3">
+    <tableColumn id="3" name="amplicon_name" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="sequence_name" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="sequence" dataDxfId="11" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <tableColumns count="7">
-    <tableColumn id="1" name="target_genome" dataDxfId="56"/>
-    <tableColumn id="2" name="strand" dataDxfId="55"/>
-    <tableColumn id="3" name="dna_feature" dataDxfId="54"/>
-    <tableColumn id="4" name="is_true_or_false" dataDxfId="53"/>
-    <tableColumn id="5" name="cell_line_name" dataDxfId="52"/>
-    <tableColumn id="6" name="content_type" dataDxfId="51"/>
-    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="50"/>
+    <tableColumn id="1" name="target_genome" dataDxfId="8"/>
+    <tableColumn id="2" name="strand" dataDxfId="7"/>
+    <tableColumn id="3" name="dna_feature" dataDxfId="6"/>
+    <tableColumn id="4" name="is_true_or_false" dataDxfId="5"/>
+    <tableColumn id="5" name="cell_line_name" dataDxfId="4"/>
+    <tableColumn id="6" name="content_type" dataDxfId="3"/>
+    <tableColumn id="7" name="sequencing_dna_source" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5065,9 +5105,9 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table466" displayName="Table466" ref="A67:C72" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="39"/>
-    <tableColumn id="2" name="Column names" dataDxfId="38"/>
-    <tableColumn id="3" name="Description" dataDxfId="37"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="125"/>
+    <tableColumn id="2" name="Column names" dataDxfId="124"/>
+    <tableColumn id="3" name="Description" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5076,9 +5116,9 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table567" displayName="Table567" ref="A23:C36" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="36"/>
-    <tableColumn id="2" name="Column names" dataDxfId="35"/>
-    <tableColumn id="3" name="Description" dataDxfId="34"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="122"/>
+    <tableColumn id="2" name="Column names" dataDxfId="121"/>
+    <tableColumn id="3" name="Description" dataDxfId="120"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5087,9 +5127,9 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table668" displayName="Table668" ref="A39:C43" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="33"/>
-    <tableColumn id="2" name="Column names" dataDxfId="32"/>
-    <tableColumn id="3" name="Description" dataDxfId="31"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="119"/>
+    <tableColumn id="2" name="Column names" dataDxfId="118"/>
+    <tableColumn id="3" name="Description" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5098,9 +5138,9 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table769" displayName="Table769" ref="A61:C66" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tab name" dataDxfId="30"/>
-    <tableColumn id="2" name="Column names" dataDxfId="29"/>
-    <tableColumn id="3" name="Description" dataDxfId="28"/>
+    <tableColumn id="1" name="Tab name" dataDxfId="116"/>
+    <tableColumn id="2" name="Column names" dataDxfId="115"/>
+    <tableColumn id="3" name="Description" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5109,20 +5149,20 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table4770" displayName="Table4770" ref="A44:C60" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="27" dataDxfId="26"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="25" dataDxfId="24"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="23" dataDxfId="22"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="113" dataDxfId="112"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="111" dataDxfId="110"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="109" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table4871" displayName="Table4871" ref="A37:C38" headerRowCount="0" totalsRowShown="0" dataDxfId="15" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table4871" displayName="Table4871" ref="A37:C38" headerRowCount="0" totalsRowShown="0" dataDxfId="107" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="21" dataDxfId="20" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="19" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="17" dataDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="106" dataDxfId="105" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="104" dataDxfId="103" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="102" dataDxfId="101" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5131,9 +5171,9 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table4972" displayName="Table4972" ref="A19:C22" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" headerRowDxfId="14" dataDxfId="13"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="12" dataDxfId="11"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="10" dataDxfId="9"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="100" dataDxfId="99"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="98" dataDxfId="97"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="96" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5466,7 +5506,7 @@
   </sheetPr>
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
@@ -6132,7 +6172,7 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6539,12 +6579,12 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -6566,48 +6606,51 @@
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6616,45 +6659,48 @@
         <v>262</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="16">
+      <c r="D2" s="16">
         <v>53704225</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>16</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="I2" s="14">
+      <c r="J2" s="14">
         <v>53704130</v>
       </c>
-      <c r="J2" s="14">
+      <c r="K2" s="14">
         <v>53704148</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="L2" s="14">
+      <c r="M2" s="14">
         <v>53704291</v>
       </c>
-      <c r="M2" s="14">
+      <c r="N2" s="14">
         <v>53704310</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="P2" s="14" t="s">
         <v>281</v>
       </c>
     </row>
@@ -6663,45 +6709,48 @@
         <v>266</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>53700682</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>16</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="I3" s="14">
+      <c r="J3" s="14">
         <v>53700624</v>
       </c>
-      <c r="J3" s="14">
+      <c r="K3" s="14">
         <v>53700643</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="L3" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="L3" s="14">
+      <c r="M3" s="14">
         <v>53700846</v>
       </c>
-      <c r="M3" s="14">
+      <c r="N3" s="14">
         <v>53700865</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="P3" s="14" t="s">
         <v>281</v>
       </c>
     </row>
@@ -6710,45 +6759,48 @@
         <v>269</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>44344558</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>2</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="I4" s="14">
+      <c r="J4" s="14">
         <v>44344474</v>
       </c>
-      <c r="J4" s="14">
+      <c r="K4" s="14">
         <v>44344498</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="L4" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="L4" s="14">
+      <c r="M4" s="14">
         <v>44344585</v>
       </c>
-      <c r="M4" s="14">
+      <c r="N4" s="14">
         <v>44344605</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="P4" s="14" t="s">
         <v>281</v>
       </c>
     </row>
@@ -6757,45 +6809,48 @@
         <v>272</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>54285883</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>16</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="I5" s="14">
+      <c r="J5" s="14">
         <v>54285780</v>
       </c>
-      <c r="J5" s="14">
+      <c r="K5" s="14">
         <v>54285799</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="L5" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="L5" s="14">
+      <c r="M5" s="14">
         <v>54285919</v>
       </c>
-      <c r="M5" s="14">
+      <c r="N5" s="14">
         <v>54285936</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="P5" s="14" t="s">
         <v>288</v>
       </c>
     </row>
@@ -6804,45 +6859,48 @@
         <v>275</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>54931241</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>16</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="I6" s="14">
+      <c r="J6" s="14">
         <v>54931181</v>
       </c>
-      <c r="J6" s="14">
+      <c r="K6" s="14">
         <v>54931195</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="L6" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="L6" s="14">
+      <c r="M6" s="14">
         <v>54931377</v>
       </c>
-      <c r="M6" s="14">
+      <c r="N6" s="14">
         <v>54931395</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="P6" s="14" t="s">
         <v>288</v>
       </c>
     </row>
@@ -6860,6 +6918,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
     </row>
     <row r="15" spans="1:18">
       <c r="C15" s="16"/>
@@ -6930,19 +6989,19 @@
           <x14:formula1>
             <xm:f>Menus!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>F10:F1048576 G2:G9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Menus!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D10:D1048576 E2:E9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Menus!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>E10:E1048576 F2:F9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11303,7 +11362,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -11312,48 +11371,60 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="136.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="121.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="20" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="20"/>
       <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" ht="15">
-      <c r="A3" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="20"/>
       <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" ht="15">
-      <c r="A4" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="20"/>
       <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" ht="15">
-      <c r="A5" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="20"/>
       <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" ht="15">
-      <c r="A6" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="20"/>
       <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" ht="15">
-      <c r="A7" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="20"/>
       <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" ht="15">
-      <c r="A8" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="20"/>
       <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" ht="15">
-      <c r="A9" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="15">
+      <c r="A9" s="20"/>
       <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>